<commit_message>
added other to adj updated template
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.5.xlsx
+++ b/Projects/GMIUS/Data/Yogurt GMI KPI Template v0.5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,6 +52,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$F$40</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$F$40</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$F$40</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$F$40</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="b" vbProcedure="false">'Anchor List'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="e" vbProcedure="false">'Anchor List'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="h" vbProcedure="false">'Anchor List'!$A$1:$I$1</definedName>
@@ -75,6 +76,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Anchor List'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Anchor List'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Anchor List'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Anchor List'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -574,7 +576,7 @@
     <t xml:space="preserve">adjacency</t>
   </si>
   <si>
-    <t xml:space="preserve">Noosa, Chobani Greek, Chobani Hint, Siggi's, Brown Cow, Greek Gods, Yoplait Traditional, Fage, Other Simply Better, Organic, Non Dairy</t>
+    <t xml:space="preserve">Noosa, Chobani Greek, Chobani Hint, Siggi's, Brown Cow, Greek Gods, Yoplait Traditional, Fage, Other Simply Better, Organic, Non Dairy, END OF CATEGORY</t>
   </si>
   <si>
     <t xml:space="preserve">KID ON LEFT, PROBIOTIC ON RIGHT; PROBIOTIC ON LEFT, KID ON RIGHT; KID ON BOTH, PROBIOTIC ON RIGHT; KID ON BOTH, PROBIOTIC ON LEFT; PRIOBIOTIC ON BOTH, KID ON RIGHT; PROBIOTIC ON BOTH, KID ON LEFT; BOTH ON LEFT; BOTH ON RIGHT; ONLY KID ON RIGHT; ONLY KID ON LEFT; ONLY KID BOTH; ONLY PROBIOTIC ON RIGHT; ONLY PROBIOTIC ON LEFT; ONLY PROBIOTIC BOTH; Neither Kid or ASH Anchors</t>
@@ -604,13 +606,13 @@
     <t xml:space="preserve">All Organic Blocked within Mainstream Yogurt Set; Adult Organic and Kid Organic Blocked Separately; Interspersed within Mainstream Yogurt Set; Blocked, Separate Location in Separate Aisle; No Distribution</t>
   </si>
   <si>
-    <t xml:space="preserve">Noosa, Oui, Chobani Hint, Siggi's, Brown Cow, Greek Gods, Yoplait Traditional, Fage, Chobani Greek, Organic, Non Dairy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noosa, YQ, Chobani Hint, Siggi's, Brown Cow, Greek Gods, Yoplait Traditional, Fage, Chobani Greek, Organic, Non Dairy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silk, So Delicious, Greek, Simply Better, Organic, Non Dairy</t>
+    <t xml:space="preserve">Noosa, Oui, Chobani Hint, Siggi's, Brown Cow, Greek Gods, Yoplait Traditional, Fage, Chobani Greek, Organic, Non Dairy, END OF CATEGORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noosa, YQ, Chobani Hint, Siggi's, Brown Cow, Greek Gods, Yoplait Traditional, Fage, Chobani Greek, Organic, Non Dairy, END OF CATEGORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silk, So Delicious, Greek, Simply Better, Organic, Non Dairy, END OF CATEGORY</t>
   </si>
   <si>
     <t xml:space="preserve">Criteria 1</t>
@@ -964,7 +966,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,7 +1733,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,12 +1801,14 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,7 +2059,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,7 +2173,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2372,7 +2376,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,13 +2425,13 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2500,7 +2504,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,12 +2583,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="88.2925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="29.1037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="90.5481481481482"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="29.7888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.54444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2885,12 +2889,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.8296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="29.1037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.5925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="29.7888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3074,13 +3078,13 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.3962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.2592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3363,14 +3367,14 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.0703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.637037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3507,13 +3511,13 @@
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X2" activeCellId="0" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>